<commit_message>
Actualización nro sprints del acta constitucion PRY con el cronograma del proyecto
</commit_message>
<xml_diff>
--- a/Cronograma_Desarrollo_y_Ejecución_PRY_SGVR.xlsx
+++ b/Cronograma_Desarrollo_y_Ejecución_PRY_SGVR.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ing_Sistemas\IngSoftwareII\REspaldosVersionesIniciales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\Grupo11_22Nov\UIsrael_IngSoftwareII_Grupo11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72287387-5A8B-4E0E-A5C9-6851785A3113}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71ACAE72-AEF1-4668-8BF1-DA338388530C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A4089093-2625-4DD9-A5FA-0B4D021EBB75}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A4089093-2625-4DD9-A5FA-0B4D021EBB75}"/>
   </bookViews>
   <sheets>
-    <sheet name="Acta_Constitucion_PRY_SGVR" sheetId="1" r:id="rId1"/>
+    <sheet name="Borrador_Cronog Constitucion Pr" sheetId="1" r:id="rId1"/>
     <sheet name="Bak_Acta_Constitucion_PRY_SGVR" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -426,7 +426,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Se sube la planificación del proyecto, tomando el reajuste de la estimacion costos por Punto Funcion.
</commit_message>
<xml_diff>
--- a/Cronograma_Desarrollo_y_Ejecución_PRY_SGVR.xlsx
+++ b/Cronograma_Desarrollo_y_Ejecución_PRY_SGVR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\GitHub\Grupo11_22Nov\UIsrael_IngSoftwareII_Grupo11\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71ACAE72-AEF1-4668-8BF1-DA338388530C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3170B25E-F160-40F6-AC39-47520F157606}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A4089093-2625-4DD9-A5FA-0B4D021EBB75}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Borrador_Cronog Constitucion Pr" sheetId="1" r:id="rId1"/>
     <sheet name="Bak_Acta_Constitucion_PRY_SGVR" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -62,7 +62,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +74,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,7 +106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -107,6 +114,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -426,13 +438,14 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -455,15 +468,15 @@
         <v>44256</v>
       </c>
       <c r="B2" s="1">
-        <v>44435</v>
+        <v>44498</v>
       </c>
       <c r="C2" s="4">
         <f>NETWORKDAYS(A2,B2)</f>
-        <v>130</v>
+        <v>175</v>
       </c>
       <c r="D2" s="4">
         <f>C2/5</f>
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -481,25 +494,25 @@
         <v>44263</v>
       </c>
       <c r="B4" s="1">
-        <v>44428</v>
+        <v>44491</v>
       </c>
       <c r="C4" s="4">
         <f>NETWORKDAYS(A4,B4)</f>
-        <v>120</v>
+        <v>165</v>
       </c>
       <c r="D4" s="4">
         <f>C4/5</f>
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E4" t="s">
         <v>7</v>
       </c>
       <c r="F4" s="4">
-        <f>D4/12</f>
-        <v>2</v>
+        <f>D4/11</f>
+        <v>3</v>
       </c>
       <c r="G4" s="4">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -519,7 +532,7 @@
       </c>
       <c r="B7" s="1">
         <f>WORKDAY.INTL(A7,$G$4,1,0)</f>
-        <v>44277</v>
+        <v>44281</v>
       </c>
       <c r="D7" s="4">
         <v>1</v>
@@ -528,11 +541,11 @@
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <f>B7+1</f>
-        <v>44278</v>
+        <v>44282</v>
       </c>
       <c r="B8" s="1">
         <f>WORKDAY.INTL(A8,$G$4,1,0)</f>
-        <v>44292</v>
+        <v>44301</v>
       </c>
       <c r="D8" s="4">
         <v>2</v>
@@ -541,11 +554,11 @@
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <f>B8+1</f>
-        <v>44293</v>
+        <v>44302</v>
       </c>
       <c r="B9" s="1">
         <f t="shared" ref="B9:B18" si="0">WORKDAY.INTL(A9,$G$4,1,0)</f>
-        <v>44307</v>
+        <v>44322</v>
       </c>
       <c r="D9" s="4">
         <v>3</v>
@@ -554,11 +567,11 @@
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <f t="shared" ref="A10:A18" si="1">B9+1</f>
-        <v>44308</v>
+        <v>44323</v>
       </c>
       <c r="B10" s="1">
         <f t="shared" si="0"/>
-        <v>44322</v>
+        <v>44343</v>
       </c>
       <c r="D10" s="4">
         <v>4</v>
@@ -567,11 +580,11 @@
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <f t="shared" si="1"/>
-        <v>44323</v>
+        <v>44344</v>
       </c>
       <c r="B11" s="1">
         <f t="shared" si="0"/>
-        <v>44337</v>
+        <v>44364</v>
       </c>
       <c r="D11" s="4">
         <v>5</v>
@@ -580,11 +593,11 @@
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <f t="shared" si="1"/>
-        <v>44338</v>
+        <v>44365</v>
       </c>
       <c r="B12" s="1">
         <f t="shared" si="0"/>
-        <v>44351</v>
+        <v>44385</v>
       </c>
       <c r="D12" s="4">
         <v>6</v>
@@ -593,11 +606,11 @@
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <f t="shared" si="1"/>
-        <v>44352</v>
+        <v>44386</v>
       </c>
       <c r="B13" s="1">
         <f t="shared" si="0"/>
-        <v>44365</v>
+        <v>44406</v>
       </c>
       <c r="D13" s="4">
         <v>7</v>
@@ -606,11 +619,11 @@
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <f t="shared" si="1"/>
-        <v>44366</v>
+        <v>44407</v>
       </c>
       <c r="B14" s="1">
         <f t="shared" si="0"/>
-        <v>44379</v>
+        <v>44427</v>
       </c>
       <c r="D14" s="4">
         <v>8</v>
@@ -619,11 +632,11 @@
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <f t="shared" si="1"/>
-        <v>44380</v>
+        <v>44428</v>
       </c>
       <c r="B15" s="1">
         <f t="shared" si="0"/>
-        <v>44393</v>
+        <v>44448</v>
       </c>
       <c r="D15" s="4">
         <v>9</v>
@@ -632,11 +645,11 @@
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <f t="shared" si="1"/>
-        <v>44394</v>
+        <v>44449</v>
       </c>
       <c r="B16" s="1">
         <f t="shared" si="0"/>
-        <v>44407</v>
+        <v>44469</v>
       </c>
       <c r="D16" s="4">
         <v>10</v>
@@ -645,26 +658,27 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <f t="shared" si="1"/>
-        <v>44408</v>
+        <v>44470</v>
       </c>
       <c r="B17" s="1">
         <f t="shared" si="0"/>
-        <v>44421</v>
+        <v>44490</v>
       </c>
       <c r="D17" s="4">
         <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <f t="shared" si="1"/>
-        <v>44422</v>
-      </c>
-      <c r="B18" s="1">
-        <f t="shared" si="0"/>
-        <v>44435</v>
-      </c>
-      <c r="D18" s="4">
+      <c r="A18" s="5">
+        <f t="shared" si="1"/>
+        <v>44491</v>
+      </c>
+      <c r="B18" s="5">
+        <f t="shared" si="0"/>
+        <v>44511</v>
+      </c>
+      <c r="C18" s="6"/>
+      <c r="D18" s="7">
         <v>12</v>
       </c>
     </row>

</xml_diff>